<commit_message>
Halfway through implementing Login.
</commit_message>
<xml_diff>
--- a/data/ApplicantList.xlsx
+++ b/data/ApplicantList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>John</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>PasswordTest</t>
+  </si>
+  <si>
+    <t>Jordan Chua</t>
+  </si>
+  <si>
+    <t>S9876555J</t>
   </si>
 </sst>
 </file>
@@ -122,7 +128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -232,10 +238,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>20</v>
@@ -244,6 +250,23 @@
         <v>8</v>
       </c>
       <c r="E7" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s" s="0">
         <v>21</v>
       </c>
     </row>

</xml_diff>